<commit_message>
Design na tabela de estatistica
</commit_message>
<xml_diff>
--- a/documentacao/Dados_Estatistica_Basica.xlsx
+++ b/documentacao/Dados_Estatistica_Basica.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia\Documents\git PI\Ar Condicionado\TechHumi\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0194308-41E9-4981-ABD2-9505708A0F1A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>Temperatura</t>
   </si>
@@ -56,20 +63,17 @@
     <t>Máximo</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Mínimo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,8 +95,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +145,122 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE66914"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF19B61"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B184"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF68A042"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF91C46E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFACD391"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3F89CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFD8EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6A8ED0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE853E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -135,16 +269,227 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -158,23 +503,207 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="21" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="19" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="16" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="16" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Ênfase5" xfId="4" builtinId="47"/>
@@ -186,6 +715,20 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3F89CD"/>
+      <color rgb="FF5899D4"/>
+      <color rgb="FF91C46E"/>
+      <color rgb="FF68A042"/>
+      <color rgb="FFF4B184"/>
+      <color rgb="FFF19B61"/>
+      <color rgb="FFE66914"/>
+      <color rgb="FFEE853E"/>
+      <color rgb="FF4472C4"/>
+      <color rgb="FF6A8ED0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -459,11 +1002,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,795 +1020,864 @@
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
         <v>26</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="15">
         <v>56</v>
       </c>
-      <c r="D3" s="4">
+      <c r="C3" s="3"/>
+      <c r="D3" s="16">
         <f>SUM(A3,2)</f>
         <v>28</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="17">
         <f>SUM(B3,1)</f>
         <v>57</v>
       </c>
-      <c r="G3" s="4">
+      <c r="F3" s="3"/>
+      <c r="G3" s="18">
         <f>SUM(A3-2)</f>
         <v>24</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="19">
         <f>SUM(B3-1)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20">
         <v>26</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="21">
         <v>57</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="4">
+      <c r="C4" s="22"/>
+      <c r="D4" s="23">
         <f t="shared" ref="D4:D22" si="0">SUM(A4,2)</f>
         <v>28</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="24">
         <f t="shared" ref="E4:E22" si="1">SUM(B4,1)</f>
         <v>58</v>
       </c>
-      <c r="G4" s="4">
+      <c r="F4" s="3"/>
+      <c r="G4" s="25">
         <f t="shared" ref="G4:G22" si="2">SUM(A4-2)</f>
         <v>24</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="26">
         <f t="shared" ref="H4:H22" si="3">SUM(B4-1)</f>
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27">
         <v>26</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="28">
         <v>59</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="4">
+      <c r="C5" s="22"/>
+      <c r="D5" s="29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="30">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G5" s="4">
+      <c r="F5" s="3"/>
+      <c r="G5" s="31">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="32">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="67"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20">
         <v>26</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="21">
         <v>59</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="4">
+      <c r="C6" s="22"/>
+      <c r="D6" s="23">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="24">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G6" s="4">
+      <c r="F6" s="3"/>
+      <c r="G6" s="25">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="26">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="44"/>
+      <c r="K6" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="O6" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="P6" s="46" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="Q6" s="67"/>
+      <c r="R6" s="67"/>
+      <c r="S6" s="67"/>
+      <c r="T6" s="67"/>
+      <c r="U6" s="67"/>
+      <c r="V6" s="67"/>
+    </row>
+    <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27">
         <v>26</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="28">
         <v>59</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="4">
+      <c r="C7" s="22"/>
+      <c r="D7" s="29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="30">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G7" s="4">
+      <c r="F7" s="3"/>
+      <c r="G7" s="31">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="32">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="49">
         <f>MIN(A3:A22)</f>
         <v>26</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="50">
         <f>QUARTILE(A3:A22,1)</f>
         <v>26</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="49">
         <f>AVERAGE(A3:A22)</f>
         <v>26.75</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="50">
         <f>MEDIAN(A3:A22)</f>
         <v>27</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="49">
         <f>QUARTILE(A3:A22,3)</f>
         <v>27</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="50">
         <f>MAX(A3:A22)</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="67"/>
+      <c r="T7" s="67"/>
+      <c r="U7" s="67"/>
+      <c r="V7" s="67"/>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20">
         <v>26</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="21">
         <v>68</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4">
+      <c r="C8" s="22"/>
+      <c r="D8" s="23">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="24">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="G8" s="4">
+      <c r="F8" s="3"/>
+      <c r="G8" s="25">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="26">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="52">
         <f>MIN(B3:B22)</f>
         <v>51</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="53">
         <f>QUARTILE(B3:B22,1)</f>
         <v>57.75</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="52">
         <f>AVERAGE(B3:B22)</f>
         <v>60.6</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="53">
         <f>MEDIAN(B3:B22)</f>
         <v>59</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="52">
         <f>QUARTILE(B3:B22,3)</f>
         <v>61.5</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="53">
         <f>MAX(B3:B22)</f>
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="67"/>
+      <c r="U8" s="67"/>
+      <c r="V8" s="67"/>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27">
         <v>26</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="28">
         <v>73</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="4">
+      <c r="C9" s="22"/>
+      <c r="D9" s="29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="30">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="G9" s="4">
+      <c r="F9" s="3"/>
+      <c r="G9" s="31">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="32">
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="67"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="67"/>
+      <c r="U9" s="67"/>
+      <c r="V9" s="67"/>
+    </row>
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20">
         <v>26</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="21">
         <v>70</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="4">
+      <c r="C10" s="22"/>
+      <c r="D10" s="23">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="24">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="G10" s="4">
+      <c r="F10" s="3"/>
+      <c r="G10" s="25">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="26">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="67"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="67"/>
+      <c r="U10" s="67"/>
+      <c r="V10" s="67"/>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27">
         <v>26</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="28">
         <v>66</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="4">
+      <c r="C11" s="22"/>
+      <c r="D11" s="29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="30">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="G11" s="4">
+      <c r="F11" s="3"/>
+      <c r="G11" s="31">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="32">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="44"/>
+      <c r="K11" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="P11" s="56" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20">
         <v>27</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="21">
         <v>63</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="4">
+      <c r="C12" s="22"/>
+      <c r="D12" s="23">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="24">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="G12" s="4">
+      <c r="F12" s="3"/>
+      <c r="G12" s="25">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="26">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="50">
         <f>MIN(D3:D22)</f>
         <v>28</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="49">
         <f>QUARTILE(D3:D22,1)</f>
         <v>28</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="50">
         <f>AVERAGE(D3:D22)</f>
         <v>28.75</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="49">
         <f>MEDIAN(D3:D22)</f>
         <v>29</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12" s="50">
         <f>QUARTILE(D3:D22,3)</f>
         <v>29</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="58">
         <f>MAX(D3:D22)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+    <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27">
         <v>27</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="28">
         <v>61</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="4">
+      <c r="C13" s="22"/>
+      <c r="D13" s="29">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="30">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="G13" s="4">
+      <c r="F13" s="3"/>
+      <c r="G13" s="31">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="32">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="53">
         <f>MIN(E3:E22)</f>
         <v>52</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="52">
         <f>QUARTILE(E3:E22,1)</f>
         <v>58.75</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="53">
         <f>AVERAGE(E3:E22)</f>
         <v>61.6</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="52">
         <f>MEDIAN(E3:E22)</f>
         <v>60</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="53">
         <f>QUARTILE(E3:E22,3)</f>
         <v>62.5</v>
       </c>
-      <c r="P13" s="5">
+      <c r="P13" s="60">
         <f>MAX(E3:E22)</f>
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+    <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20">
         <v>27</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="21">
         <v>60</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="4">
+      <c r="C14" s="22"/>
+      <c r="D14" s="23">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="24">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="G14" s="4">
+      <c r="F14" s="3"/>
+      <c r="G14" s="25">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="26">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27">
         <v>27</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="28">
         <v>59</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="4">
+      <c r="C15" s="22"/>
+      <c r="D15" s="29">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="30">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G15" s="4">
+      <c r="F15" s="3"/>
+      <c r="G15" s="31">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="32">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="43"/>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20">
         <v>27</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="21">
         <v>58</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="4">
+      <c r="C16" s="22"/>
+      <c r="D16" s="23">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="24">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="G16" s="4">
+      <c r="F16" s="3"/>
+      <c r="G16" s="25">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="26">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="44"/>
+      <c r="K16" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16" s="6" t="s">
+      <c r="L16" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="M16" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="N16" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="6" t="s">
+      <c r="O16" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="P16" s="6" t="s">
+      <c r="P16" s="65" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27">
         <v>27</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="28">
         <v>61</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="4">
+      <c r="C17" s="22"/>
+      <c r="D17" s="29">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="30">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="G17" s="4">
+      <c r="F17" s="3"/>
+      <c r="G17" s="31">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="32">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="49">
         <f>MIN(G3:G22)</f>
         <v>24</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="50">
         <f>QUARTILE(G3:G22,1)</f>
         <v>24</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="50">
         <f>AVERAGE(G3:G22)</f>
         <v>24.75</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="49">
         <f>MEDIAN(G3:G22)</f>
         <v>25</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17" s="50">
         <f>QUARTILE(G3:G22,3)</f>
         <v>25</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17" s="58">
         <f>MAX(G3:G22)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20">
         <v>28</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="21">
         <v>60</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="4">
+      <c r="C18" s="22"/>
+      <c r="D18" s="23">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="24">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="G18" s="4">
+      <c r="F18" s="3"/>
+      <c r="G18" s="25">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="26">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="52">
         <f>MIN(H3:H22)</f>
         <v>50</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="53">
         <f>QUARTILE(H3:H22,1)</f>
         <v>56.75</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="53">
         <f>AVERAGE(H3:H22)</f>
         <v>59.6</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="52">
         <f>MEDIAN(H3:H22)</f>
         <v>58</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="53">
         <f>QUARTILE(H3:H22,3)</f>
         <v>60.5</v>
       </c>
-      <c r="P18" s="5">
+      <c r="P18" s="60">
         <f>MAX(H3:H22)</f>
         <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="27">
         <v>28</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="28">
         <v>59</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="4">
+      <c r="C19" s="22"/>
+      <c r="D19" s="29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="30">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G19" s="4">
+      <c r="F19" s="3"/>
+      <c r="G19" s="31">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="32">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="20">
         <v>28</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="21">
         <v>57</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="4">
+      <c r="C20" s="22"/>
+      <c r="D20" s="23">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="24">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="G20" s="4">
+      <c r="F20" s="3"/>
+      <c r="G20" s="25">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="26">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="27">
         <v>28</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="28">
         <v>56</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="4">
+      <c r="C21" s="22"/>
+      <c r="D21" s="29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="30">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="G21" s="4">
+      <c r="F21" s="3"/>
+      <c r="G21" s="31">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="32">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="33">
         <v>27</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="34">
         <v>51</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="4">
+      <c r="C22" s="22"/>
+      <c r="D22" s="35">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="36">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="G22" s="4">
+      <c r="F22" s="3"/>
+      <c r="G22" s="37">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="38">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
@@ -1280,5 +1892,6 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>